<commit_message>
Refactor: rename 'manufactured death' to 'structural barriers'
- Updated all Python files to use 'Structural Barriers' terminology
- Renamed ManufacturedDeathModel class to StructuralBarrierModel
- Updated output filenames from manufactured_death_results to structural_barrier_results
- Added new supplementary figures for preprints.org submission
- Added sn-vancouver-num.bst citation style file
- Removed deprecated architectural_barrier_model.py
- Moved deprecated output files to legacy/deprecated_outputs/

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/csv_xlsx/stochastic_avoidance_sensitivity_results.xlsx
+++ b/data/csv_xlsx/stochastic_avoidance_sensitivity_results.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3">
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>98</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="4">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.98</v>
+        <v>0.9715</v>
       </c>
     </row>
     <row r="5">
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.836734693877551</v>
+        <v>3.792074112197632</v>
       </c>
     </row>
     <row r="7">
@@ -505,7 +505,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3.911505471306622</v>
+        <v>3.709746932931708</v>
       </c>
     </row>
     <row r="8">
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5.75</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -545,7 +545,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.7448979591836735</v>
+        <v>0.7380339680905815</v>
       </c>
     </row>
     <row r="13">
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9081632653061225</v>
+        <v>0.9274318064848173</v>
       </c>
     </row>
   </sheetData>
@@ -629,16 +629,16 @@
         <v>1000</v>
       </c>
       <c r="C2" t="n">
-        <v>986</v>
+        <v>976</v>
       </c>
       <c r="D2" t="n">
-        <v>0.986</v>
+        <v>0.976</v>
       </c>
       <c r="E2" t="n">
         <v>2</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7809330628803245</v>
+        <v>0.7838114754098361</v>
       </c>
     </row>
     <row r="3">
@@ -651,16 +651,16 @@
         <v>1000</v>
       </c>
       <c r="C3" t="n">
-        <v>992</v>
+        <v>996</v>
       </c>
       <c r="D3" t="n">
-        <v>0.992</v>
+        <v>0.996</v>
       </c>
       <c r="E3" t="n">
         <v>2</v>
       </c>
       <c r="F3" t="n">
-        <v>0.875</v>
+        <v>0.8634538152610441</v>
       </c>
     </row>
     <row r="4">
@@ -673,16 +673,16 @@
         <v>1000</v>
       </c>
       <c r="C4" t="n">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="D4" t="n">
-        <v>0.99</v>
+        <v>0.988</v>
       </c>
       <c r="E4" t="n">
         <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7767676767676768</v>
+        <v>0.7834008097165992</v>
       </c>
     </row>
     <row r="5">
@@ -695,16 +695,16 @@
         <v>1000</v>
       </c>
       <c r="C5" t="n">
-        <v>968</v>
+        <v>971</v>
       </c>
       <c r="D5" t="n">
-        <v>0.968</v>
+        <v>0.971</v>
       </c>
       <c r="E5" t="n">
         <v>3</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7355371900826446</v>
+        <v>0.7250257466529351</v>
       </c>
     </row>
   </sheetData>
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7286742034943474</v>
+        <v>0.6953846153846154</v>
       </c>
       <c r="C2" t="n">
         <v>3</v>
@@ -779,7 +779,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.6787620064034151</v>
+        <v>0.6764091858037579</v>
       </c>
       <c r="C3" t="n">
         <v>3</v>
@@ -798,10 +798,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.6649214659685864</v>
+        <v>0.700312174817898</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
         <v>0.21</v>
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6331550802139038</v>
+        <v>0.6189451022604952</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
@@ -836,7 +836,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.6392199349945829</v>
+        <v>0.6434782608695652</v>
       </c>
       <c r="C6" t="n">
         <v>4</v>
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.5424757281553398</v>
+        <v>0.5082382762991128</v>
       </c>
       <c r="C7" t="n">
         <v>5</v>
@@ -915,13 +915,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7355197524528831</v>
+        <v>0.7304657182353299</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6595804988662132</v>
+        <v>0.6353124999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8119999999999999</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="3">
@@ -931,13 +931,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9311347035268008</v>
+        <v>0.9252023740057934</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8984230055658627</v>
+        <v>0.8699343434343434</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9753510638297872</v>
+        <v>0.9696969696969697</v>
       </c>
     </row>
     <row r="4">
@@ -947,13 +947,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2.6</v>
+        <v>2.782</v>
       </c>
       <c r="C4" t="n">
         <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>3.549999999999999</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>